<commit_message>
bump on-board assignment iteration
skip-ci
</commit_message>
<xml_diff>
--- a/notebooks/on-board-assign-parameter-calibration-log.xlsx
+++ b/notebooks/on-board-assign-parameter-calibration-log.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsp/Documents/GitHub/tm2py/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC4D40E-0755-624B-985A-FD7A773E9823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF967561-53D5-934A-828C-9AF5F671B1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25840" yWindow="2940" windowWidth="23160" windowHeight="17440" xr2:uid="{178A1E19-C433-0046-8576-F58438D89C43}"/>
+    <workbookView xWindow="7120" yWindow="500" windowWidth="43100" windowHeight="23340" xr2:uid="{178A1E19-C433-0046-8576-F58438D89C43}"/>
   </bookViews>
   <sheets>
     <sheet name="iter_02" sheetId="1" r:id="rId1"/>
     <sheet name="iter_04" sheetId="2" r:id="rId2"/>
+    <sheet name="iter_05" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
   <si>
     <t>parameter</t>
   </si>
@@ -94,7 +95,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,6 +123,11 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -162,6 +168,12 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -500,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0038F0A-C8EB-7340-AC40-0FBA1A6789C8}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEBE3EC5-7ED5-4440-B702-F12BEF2A035E}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,4 +960,231 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{522D5BC0-F364-0E44-88E6-252E378E6217}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="8" width="20.83203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.9</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.7</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>3</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5">
+        <v>3</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8">
+        <v>2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8">
+        <v>2</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bump pathbuilder calibration versions
</commit_message>
<xml_diff>
--- a/notebooks/on-board-assign-parameter-calibration-log.xlsx
+++ b/notebooks/on-board-assign-parameter-calibration-log.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wsp/Documents/GitHub/tm2py/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF967561-53D5-934A-828C-9AF5F671B1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65111D68-A9D0-1847-940C-07A8DFD829EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7120" yWindow="500" windowWidth="43100" windowHeight="23340" xr2:uid="{178A1E19-C433-0046-8576-F58438D89C43}"/>
+    <workbookView xWindow="11440" yWindow="2800" windowWidth="37820" windowHeight="23340" activeTab="3" xr2:uid="{178A1E19-C433-0046-8576-F58438D89C43}"/>
   </bookViews>
   <sheets>
     <sheet name="iter_02" sheetId="1" r:id="rId1"/>
     <sheet name="iter_04" sheetId="2" r:id="rId2"/>
     <sheet name="iter_05" sheetId="3" r:id="rId3"/>
+    <sheet name="iter_06" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="16">
   <si>
     <t>parameter</t>
   </si>
@@ -95,7 +96,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -128,6 +129,12 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="0"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -174,6 +181,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -512,17 +526,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0038F0A-C8EB-7340-AC40-0FBA1A6789C8}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.5" customWidth="1"/>
     <col min="2" max="8" width="20.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +562,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="30" customHeight="1">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -574,7 +588,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" customHeight="1">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -600,7 +614,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" customHeight="1">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -626,7 +640,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" customHeight="1">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -652,7 +666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" customHeight="1">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -678,7 +692,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="30" customHeight="1">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -704,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -743,13 +757,13 @@
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.5" customWidth="1"/>
     <col min="2" max="8" width="20.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="30" customHeight="1">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -801,7 +815,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" customHeight="1">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -827,7 +841,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" customHeight="1">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -853,7 +867,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" customHeight="1">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -879,7 +893,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" customHeight="1">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -905,7 +919,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="30" customHeight="1">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -931,7 +945,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -970,13 +984,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="29.5" customWidth="1"/>
     <col min="2" max="8" width="20.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +1016,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="30" customHeight="1">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1028,7 +1042,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="30" customHeight="1">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -1054,7 +1068,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="30" customHeight="1">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1094,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="30" customHeight="1">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1106,7 +1120,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" ht="30" customHeight="1">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1132,7 +1146,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="30" customHeight="1">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1158,7 +1172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" ht="30" customHeight="1">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1181,6 +1195,233 @@
         <v>15</v>
       </c>
       <c r="H8" s="5">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{689D9171-F56A-D74E-94E4-7C7095E06056}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="29.5" customWidth="1"/>
+    <col min="2" max="8" width="20.83203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="30" customHeight="1">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30" customHeight="1">
+      <c r="A2" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="F2" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="G2" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1">
+      <c r="A3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="12">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>3</v>
+      </c>
+      <c r="F3" s="6">
+        <v>3</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30" customHeight="1">
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2</v>
+      </c>
+      <c r="D4" s="12">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>3</v>
+      </c>
+      <c r="G4" s="12">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1">
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30" customHeight="1">
+      <c r="A6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" customHeight="1">
+      <c r="A7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1">
+      <c r="A8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6">
         <v>2</v>
       </c>
     </row>

</xml_diff>